<commit_message>
cleaned up Null vals more, added more info to table, fixed code errors
</commit_message>
<xml_diff>
--- a/PotentialData/AirportRankings2022.xlsx
+++ b/PotentialData/AirportRankings2022.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lucystorts/Desktop/BYU/Stat386/386Project/PotentialData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C3BC1EE-0D01-F840-9BAF-49CE7830236D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9571152A-8479-8C4B-92EB-9CA0F90A31D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="26680" windowHeight="16460" tabRatio="632" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -188,478 +188,478 @@
     <t>San Antonio, TX: San Antonio International</t>
   </si>
   <si>
+    <t>Indianapolis, IN: Indianapolis International</t>
+  </si>
+  <si>
+    <t>Kahului, HI: Kahului Airport</t>
+  </si>
+  <si>
+    <t>Pittsburgh, PA: Pittsburgh International</t>
+  </si>
+  <si>
+    <t>Cincinnati, OH: Cincinnati/Northern Kentucky International</t>
+  </si>
+  <si>
+    <t>Columbus, OH: John Glenn Columbus International</t>
+  </si>
+  <si>
+    <t>West Palm Beach/Palm Beach, FL: Palm Beach International</t>
+  </si>
+  <si>
+    <t>Jacksonville, FL: Jacksonville International</t>
+  </si>
+  <si>
+    <t>Burbank, CA: Bob Hope</t>
+  </si>
+  <si>
+    <t>Hartford, CT: Bradley International</t>
+  </si>
+  <si>
+    <t>Ontario, CA: Ontario International</t>
+  </si>
+  <si>
+    <t>Milwaukee, WI: General Mitchell International</t>
+  </si>
+  <si>
+    <t>Charleston, SC: Charleston AFB/International</t>
+  </si>
+  <si>
+    <t>Anchorage, AK: Ted Stevens Anchorage International</t>
+  </si>
+  <si>
+    <t>Albuquerque, NM: Albuquerque International Sunport</t>
+  </si>
+  <si>
+    <t>Boise, ID: Boise Air Terminal</t>
+  </si>
+  <si>
+    <t>Omaha, NE: Eppley Airfield</t>
+  </si>
+  <si>
+    <t>Memphis, TN: Memphis International</t>
+  </si>
+  <si>
+    <t>Reno, NV: Reno/Tahoe International</t>
+  </si>
+  <si>
+    <t>Norfolk, VA: Norfolk International</t>
+  </si>
+  <si>
+    <t>Richmond, VA: Richmond International</t>
+  </si>
+  <si>
+    <t>Kona, HI: Ellison Onizuka Kona International at Keahole</t>
+  </si>
+  <si>
+    <t>Buffalo, NY: Buffalo Niagara International</t>
+  </si>
+  <si>
+    <t>Oklahoma City, OK: Will Rogers World</t>
+  </si>
+  <si>
+    <t>Sarasota/Bradenton, FL: Sarasota/Bradenton International</t>
+  </si>
+  <si>
+    <t>Spokane, WA: Spokane International</t>
+  </si>
+  <si>
+    <t>Louisville, KY: Louisville Muhammad Ali International</t>
+  </si>
+  <si>
+    <t>El Paso, TX: El Paso International</t>
+  </si>
+  <si>
+    <t>Lihue, HI: Lihue Airport</t>
+  </si>
+  <si>
+    <t>Savannah, GA: Savannah/Hilton Head International</t>
+  </si>
+  <si>
+    <t>Grand Rapids, MI: Gerald R. Ford International</t>
+  </si>
+  <si>
+    <t>Myrtle Beach, SC: Myrtle Beach International</t>
+  </si>
+  <si>
+    <t>Tucson, AZ: Tucson International</t>
+  </si>
+  <si>
+    <t>Long Beach, CA: Long Beach Airport</t>
+  </si>
+  <si>
+    <t>Providence, RI: Rhode Island Tf Green International</t>
+  </si>
+  <si>
+    <t>Palm Springs, CA: Palm Springs International</t>
+  </si>
+  <si>
+    <t>Tulsa, OK: Tulsa International</t>
+  </si>
+  <si>
+    <t>Des Moines, IA: Des Moines International</t>
+  </si>
+  <si>
+    <t>Sanford, FL: Orlando Sanford International</t>
+  </si>
+  <si>
+    <t>Birmingham, AL: Birmingham-Shuttlesworth International</t>
+  </si>
+  <si>
+    <t>Albany, NY: Albany International</t>
+  </si>
+  <si>
+    <t>Syracuse, NY: Syracuse Hancock International</t>
+  </si>
+  <si>
+    <t>Pensacola, FL: Pensacola International</t>
+  </si>
+  <si>
+    <t>Knoxville, TN: McGhee Tyson</t>
+  </si>
+  <si>
+    <t>St. Petersburg, FL: St Pete Clearwater International</t>
+  </si>
+  <si>
+    <t>Rochester, NY: Frederick Douglass Grtr Rochester International</t>
+  </si>
+  <si>
+    <t>Bozeman, MT: Bozeman Yellowstone International</t>
+  </si>
+  <si>
+    <t>Fresno, CA: Fresno Yosemite International</t>
+  </si>
+  <si>
+    <t>Colorado Springs, CO: City of Colorado Springs Municipal</t>
+  </si>
+  <si>
+    <t>Greer, SC: Greenville-Spartanburg International</t>
+  </si>
+  <si>
+    <t>Valparaiso, FL: Eglin AFB Destin Fort Walton Beach</t>
+  </si>
+  <si>
+    <t>Portland, ME: Portland International Jetport</t>
+  </si>
+  <si>
+    <t>Little Rock, AR: Bill and Hillary Clinton Nat Adams Field</t>
+  </si>
+  <si>
+    <t>Phoenix, AZ: Phoenix - Mesa Gateway</t>
+  </si>
+  <si>
+    <t>Punta Gorda, FL: Punta Gorda Airport</t>
+  </si>
+  <si>
+    <t>Asheville, NC: Asheville Regional</t>
+  </si>
+  <si>
+    <t>Madison, WI: Dane County Regional-Truax Field</t>
+  </si>
+  <si>
+    <t>White Plains, NY: Westchester County</t>
+  </si>
+  <si>
+    <t>Fayetteville, AR: Northwest Arkansas National</t>
+  </si>
+  <si>
+    <t>Greensboro/High Point, NC: Piedmont Triad International</t>
+  </si>
+  <si>
+    <t>Eugene, OR: Mahlon Sweet Field</t>
+  </si>
+  <si>
+    <t>Wichita, KS: Wichita Dwight D Eisenhower National</t>
+  </si>
+  <si>
+    <t>Panama City, FL: Northwest Florida Beaches International</t>
+  </si>
+  <si>
+    <t>Key West, FL: Key West International</t>
+  </si>
+  <si>
+    <t>Manchester, NH: Manchester Boston Regional</t>
+  </si>
+  <si>
+    <t>Hilo, HI: Hilo International</t>
+  </si>
+  <si>
+    <t>Midland/Odessa, TX: Midland International Air and Space Port</t>
+  </si>
+  <si>
+    <t>Harrisburg, PA: Harrisburg International</t>
+  </si>
+  <si>
+    <t>Islip, NY: Long Island MacArthur</t>
+  </si>
+  <si>
+    <t>Santa Barbara, CA: Santa Barbara Municipal</t>
+  </si>
+  <si>
+    <t>Cedar Rapids/Iowa City, IA: The Eastern Iowa</t>
+  </si>
+  <si>
+    <t>Sioux Falls, SD: Joe Foss Field</t>
+  </si>
+  <si>
+    <t>Burlington, VT: Burlington International</t>
+  </si>
+  <si>
+    <t>Jackson/Vicksburg, MS: Jackson Medgar Wiley Evers International</t>
+  </si>
+  <si>
+    <t>Huntsville, AL: Huntsville International-Carl T Jones Field</t>
+  </si>
+  <si>
+    <t>Lexington, KY: Blue Grass</t>
+  </si>
+  <si>
+    <t>Dayton, OH: James M Cox/Dayton International</t>
+  </si>
+  <si>
+    <t>Springfield, MO: Springfield-Branson National</t>
+  </si>
+  <si>
+    <t>Wilmington, NC: Wilmington International</t>
+  </si>
+  <si>
+    <t>Bend/Redmond, OR: Roberts Field</t>
+  </si>
+  <si>
+    <t>Medford, OR: Rogue Valley International - Medford</t>
+  </si>
+  <si>
+    <t>Fairbanks, AK: Fairbanks International</t>
+  </si>
+  <si>
+    <t>Columbia, SC: Columbia Metropolitan</t>
+  </si>
+  <si>
+    <t>Lubbock, TX: Lubbock Preston Smith International</t>
+  </si>
+  <si>
+    <t>Fargo, ND: Hector International</t>
+  </si>
+  <si>
+    <t>Mission/McAllen/Edinburg, TX: McAllen Miller International</t>
+  </si>
+  <si>
+    <t>Harlingen/San Benito, TX: Valley International</t>
+  </si>
+  <si>
+    <t>Chattanooga, TN: Lovell Field</t>
+  </si>
+  <si>
+    <t>Missoula, MT: Missoula Montana</t>
+  </si>
+  <si>
+    <t>Kalispell, MT: Glacier Park International</t>
+  </si>
+  <si>
+    <t>Allentown/Bethlehem/Easton, PA: Lehigh Valley International</t>
+  </si>
+  <si>
+    <t>Appleton, WI: Appleton International</t>
+  </si>
+  <si>
+    <t>Atlantic City, NJ: Atlantic City International</t>
+  </si>
+  <si>
+    <t>Jackson, WY: Jackson Hole</t>
+  </si>
+  <si>
+    <t>Tallahassee, FL: Tallahassee International</t>
+  </si>
+  <si>
+    <t>Billings, MT: Billings Logan International</t>
+  </si>
+  <si>
+    <t>Juneau, AK: Juneau International</t>
+  </si>
+  <si>
+    <t>Amarillo, TX: Rick Husband Amarillo International</t>
+  </si>
+  <si>
+    <t>Fort Wayne, IN: Fort Wayne International</t>
+  </si>
+  <si>
+    <t>South Bend, IN: South Bend International</t>
+  </si>
+  <si>
+    <t>New Haven, CT: Tweed New Haven</t>
+  </si>
+  <si>
+    <t>Bangor, ME: Bangor International</t>
+  </si>
+  <si>
+    <t>Rapid City, SD: Rapid City Regional</t>
+  </si>
+  <si>
+    <t>Trenton, NJ: Trenton Mercer</t>
+  </si>
+  <si>
+    <t>Baton Rouge, LA: Baton Rouge Metropolitan/Ryan Field</t>
+  </si>
+  <si>
+    <t>Bellingham, WA: Bellingham International</t>
+  </si>
+  <si>
+    <t>Corpus Christi, TX: Corpus Christi International</t>
+  </si>
+  <si>
+    <t>Idaho Falls, ID: Idaho Falls Regional</t>
+  </si>
+  <si>
+    <t>Santa Rosa, CA: Charles M. Schulz - Sonoma County</t>
+  </si>
+  <si>
+    <t>Aspen, CO: Aspen Pitkin County Sardy Field</t>
+  </si>
+  <si>
+    <t>Flint, MI: Bishop International</t>
+  </si>
+  <si>
+    <t>Roanoke, VA: Roanoke Blacksburg Regional</t>
+  </si>
+  <si>
+    <t>Green Bay, WI: Green Bay Austin Straubel International</t>
+  </si>
+  <si>
+    <t>Traverse City, MI: Cherry Capital</t>
+  </si>
+  <si>
+    <t>Peoria, IL: General Downing - Peoria International</t>
+  </si>
+  <si>
+    <t>Daytona Beach, FL: Daytona Beach International</t>
+  </si>
+  <si>
+    <t>San Luis Obispo, CA: San Luis County Regional</t>
+  </si>
+  <si>
+    <t>Shreveport, LA: Shreveport Regional</t>
+  </si>
+  <si>
+    <t>Moline, IL: Quad Cities International</t>
+  </si>
+  <si>
+    <t>Augusta, GA: Augusta Regional at Bush Field</t>
+  </si>
+  <si>
+    <t>Akron, OH: Akron-Canton Regional</t>
+  </si>
+  <si>
+    <t>Gainesville, FL: Gainesville Regional</t>
+  </si>
+  <si>
+    <t>Mobile, AL: Mobile Regional</t>
+  </si>
+  <si>
+    <t>Everett, WA: Snohomish County</t>
+  </si>
+  <si>
+    <t>Charlottesville, VA: Charlottesville Albemarle</t>
+  </si>
+  <si>
+    <t>Gulfport/Biloxi, MS: Gulfport-Biloxi International</t>
+  </si>
+  <si>
+    <t>Bismarck/Mandan, ND: Bismarck Municipal</t>
+  </si>
+  <si>
+    <t>Montrose/Delta, CO: Montrose Regional</t>
+  </si>
+  <si>
+    <t>Lafayette, LA: Lafayette Regional Paul Fournet Field</t>
+  </si>
+  <si>
+    <t>Monterey, CA: Monterey Regional</t>
+  </si>
+  <si>
+    <t>Grand Junction, CO: Grand Junction Regional</t>
+  </si>
+  <si>
+    <t>Melbourne, FL: Melbourne Orlando International</t>
+  </si>
+  <si>
+    <t>Eagle, CO: Eagle County Regional</t>
+  </si>
+  <si>
+    <t>Provo, UT: Provo Municipal</t>
+  </si>
+  <si>
+    <t>Hayden, CO: Yampa Valley</t>
+  </si>
+  <si>
+    <t>Scranton/Wilkes-Barre, PA: Wilkes Barre Scranton International</t>
+  </si>
+  <si>
+    <t>Durango, CO: Durango La Plata County</t>
+  </si>
+  <si>
+    <t>Bloomington/Normal, IL: Central Il Regional Airport at Bloomington</t>
+  </si>
+  <si>
+    <t>Fayetteville, NC: Fayetteville Regional/Grannis Field</t>
+  </si>
+  <si>
+    <t>Charleston/Dunbar, WV: West Virginia International Yeager</t>
+  </si>
+  <si>
+    <t>Belleville, IL: Scott AFB MidAmerica St Louis</t>
+  </si>
+  <si>
+    <t>Evansville, IN: Evansville Regional</t>
+  </si>
+  <si>
+    <t>Montgomery, AL: Montgomery Regional</t>
+  </si>
+  <si>
+    <t>Newburgh/Poughkeepsie, NY: New York Stewart International</t>
+  </si>
+  <si>
+    <t>Columbus, OH: Rickenbacker International</t>
+  </si>
+  <si>
+    <t>Ketchikan, AK: Ketchikan International</t>
+  </si>
+  <si>
+    <t>Great Falls, MT: Great Falls International</t>
+  </si>
+  <si>
+    <t>Bakersfield, CA: Meadows Field</t>
+  </si>
+  <si>
+    <t>Minot, ND: Minot International</t>
+  </si>
+  <si>
+    <t>Jacksonville/Camp Lejeune, NC: Albert J Ellis</t>
+  </si>
+  <si>
+    <t>Nantucket, MA: Nantucket Memorial</t>
+  </si>
+  <si>
+    <t>Bethel, AK: Bethel Airport</t>
+  </si>
+  <si>
+    <t>St. George, UT: St George Regional</t>
+  </si>
+  <si>
+    <t>Source: Bureau of Transportation Statistics, T-100 Market</t>
+  </si>
+  <si>
+    <t>* Systemwide equals domestic plus international</t>
+  </si>
+  <si>
+    <t>Note: Percentage changes based on numbers prior to rounding.</t>
+  </si>
+  <si>
+    <t>Pasco/Kennewick/Richland, WA: Tri Cities WA</t>
+  </si>
+  <si>
+    <t>Bristol/Johnson City/Kingsport, TN: Tri Cities TN</t>
+  </si>
+  <si>
     <t>Cleveland, OH: Cleveland-Hopkins International</t>
-  </si>
-  <si>
-    <t>Indianapolis, IN: Indianapolis International</t>
-  </si>
-  <si>
-    <t>Kahului, HI: Kahului Airport</t>
-  </si>
-  <si>
-    <t>Pittsburgh, PA: Pittsburgh International</t>
-  </si>
-  <si>
-    <t>Cincinnati, OH: Cincinnati/Northern Kentucky International</t>
-  </si>
-  <si>
-    <t>Columbus, OH: John Glenn Columbus International</t>
-  </si>
-  <si>
-    <t>West Palm Beach/Palm Beach, FL: Palm Beach International</t>
-  </si>
-  <si>
-    <t>Jacksonville, FL: Jacksonville International</t>
-  </si>
-  <si>
-    <t>Burbank, CA: Bob Hope</t>
-  </si>
-  <si>
-    <t>Hartford, CT: Bradley International</t>
-  </si>
-  <si>
-    <t>Ontario, CA: Ontario International</t>
-  </si>
-  <si>
-    <t>Milwaukee, WI: General Mitchell International</t>
-  </si>
-  <si>
-    <t>Charleston, SC: Charleston AFB/International</t>
-  </si>
-  <si>
-    <t>Anchorage, AK: Ted Stevens Anchorage International</t>
-  </si>
-  <si>
-    <t>Albuquerque, NM: Albuquerque International Sunport</t>
-  </si>
-  <si>
-    <t>Boise, ID: Boise Air Terminal</t>
-  </si>
-  <si>
-    <t>Omaha, NE: Eppley Airfield</t>
-  </si>
-  <si>
-    <t>Memphis, TN: Memphis International</t>
-  </si>
-  <si>
-    <t>Reno, NV: Reno/Tahoe International</t>
-  </si>
-  <si>
-    <t>Norfolk, VA: Norfolk International</t>
-  </si>
-  <si>
-    <t>Richmond, VA: Richmond International</t>
-  </si>
-  <si>
-    <t>Kona, HI: Ellison Onizuka Kona International at Keahole</t>
-  </si>
-  <si>
-    <t>Buffalo, NY: Buffalo Niagara International</t>
-  </si>
-  <si>
-    <t>Oklahoma City, OK: Will Rogers World</t>
-  </si>
-  <si>
-    <t>Sarasota/Bradenton, FL: Sarasota/Bradenton International</t>
-  </si>
-  <si>
-    <t>Spokane, WA: Spokane International</t>
-  </si>
-  <si>
-    <t>Louisville, KY: Louisville Muhammad Ali International</t>
-  </si>
-  <si>
-    <t>El Paso, TX: El Paso International</t>
-  </si>
-  <si>
-    <t>Lihue, HI: Lihue Airport</t>
-  </si>
-  <si>
-    <t>Savannah, GA: Savannah/Hilton Head International</t>
-  </si>
-  <si>
-    <t>Grand Rapids, MI: Gerald R. Ford International</t>
-  </si>
-  <si>
-    <t>Myrtle Beach, SC: Myrtle Beach International</t>
-  </si>
-  <si>
-    <t>Tucson, AZ: Tucson International</t>
-  </si>
-  <si>
-    <t>Long Beach, CA: Long Beach Airport</t>
-  </si>
-  <si>
-    <t>Providence, RI: Rhode Island Tf Green International</t>
-  </si>
-  <si>
-    <t>Palm Springs, CA: Palm Springs International</t>
-  </si>
-  <si>
-    <t>Tulsa, OK: Tulsa International</t>
-  </si>
-  <si>
-    <t>Des Moines, IA: Des Moines International</t>
-  </si>
-  <si>
-    <t>Sanford, FL: Orlando Sanford International</t>
-  </si>
-  <si>
-    <t>Birmingham, AL: Birmingham-Shuttlesworth International</t>
-  </si>
-  <si>
-    <t>Albany, NY: Albany International</t>
-  </si>
-  <si>
-    <t>Syracuse, NY: Syracuse Hancock International</t>
-  </si>
-  <si>
-    <t>Pensacola, FL: Pensacola International</t>
-  </si>
-  <si>
-    <t>Knoxville, TN: McGhee Tyson</t>
-  </si>
-  <si>
-    <t>St. Petersburg, FL: St Pete Clearwater International</t>
-  </si>
-  <si>
-    <t>Rochester, NY: Frederick Douglass Grtr Rochester International</t>
-  </si>
-  <si>
-    <t>Bozeman, MT: Bozeman Yellowstone International</t>
-  </si>
-  <si>
-    <t>Fresno, CA: Fresno Yosemite International</t>
-  </si>
-  <si>
-    <t>Colorado Springs, CO: City of Colorado Springs Municipal</t>
-  </si>
-  <si>
-    <t>Greer, SC: Greenville-Spartanburg International</t>
-  </si>
-  <si>
-    <t>Valparaiso, FL: Eglin AFB Destin Fort Walton Beach</t>
-  </si>
-  <si>
-    <t>Portland, ME: Portland International Jetport</t>
-  </si>
-  <si>
-    <t>Little Rock, AR: Bill and Hillary Clinton Nat Adams Field</t>
-  </si>
-  <si>
-    <t>Phoenix, AZ: Phoenix - Mesa Gateway</t>
-  </si>
-  <si>
-    <t>Punta Gorda, FL: Punta Gorda Airport</t>
-  </si>
-  <si>
-    <t>Asheville, NC: Asheville Regional</t>
-  </si>
-  <si>
-    <t>Madison, WI: Dane County Regional-Truax Field</t>
-  </si>
-  <si>
-    <t>White Plains, NY: Westchester County</t>
-  </si>
-  <si>
-    <t>Fayetteville, AR: Northwest Arkansas National</t>
-  </si>
-  <si>
-    <t>Greensboro/High Point, NC: Piedmont Triad International</t>
-  </si>
-  <si>
-    <t>Eugene, OR: Mahlon Sweet Field</t>
-  </si>
-  <si>
-    <t>Wichita, KS: Wichita Dwight D Eisenhower National</t>
-  </si>
-  <si>
-    <t>Panama City, FL: Northwest Florida Beaches International</t>
-  </si>
-  <si>
-    <t>Key West, FL: Key West International</t>
-  </si>
-  <si>
-    <t>Manchester, NH: Manchester Boston Regional</t>
-  </si>
-  <si>
-    <t>Hilo, HI: Hilo International</t>
-  </si>
-  <si>
-    <t>Midland/Odessa, TX: Midland International Air and Space Port</t>
-  </si>
-  <si>
-    <t>Harrisburg, PA: Harrisburg International</t>
-  </si>
-  <si>
-    <t>Islip, NY: Long Island MacArthur</t>
-  </si>
-  <si>
-    <t>Santa Barbara, CA: Santa Barbara Municipal</t>
-  </si>
-  <si>
-    <t>Cedar Rapids/Iowa City, IA: The Eastern Iowa</t>
-  </si>
-  <si>
-    <t>Sioux Falls, SD: Joe Foss Field</t>
-  </si>
-  <si>
-    <t>Burlington, VT: Burlington International</t>
-  </si>
-  <si>
-    <t>Jackson/Vicksburg, MS: Jackson Medgar Wiley Evers International</t>
-  </si>
-  <si>
-    <t>Huntsville, AL: Huntsville International-Carl T Jones Field</t>
-  </si>
-  <si>
-    <t>Lexington, KY: Blue Grass</t>
-  </si>
-  <si>
-    <t>Dayton, OH: James M Cox/Dayton International</t>
-  </si>
-  <si>
-    <t>Springfield, MO: Springfield-Branson National</t>
-  </si>
-  <si>
-    <t>Wilmington, NC: Wilmington International</t>
-  </si>
-  <si>
-    <t>Bend/Redmond, OR: Roberts Field</t>
-  </si>
-  <si>
-    <t>Medford, OR: Rogue Valley International - Medford</t>
-  </si>
-  <si>
-    <t>Fairbanks, AK: Fairbanks International</t>
-  </si>
-  <si>
-    <t>Columbia, SC: Columbia Metropolitan</t>
-  </si>
-  <si>
-    <t>Lubbock, TX: Lubbock Preston Smith International</t>
-  </si>
-  <si>
-    <t>Fargo, ND: Hector International</t>
-  </si>
-  <si>
-    <t>Mission/McAllen/Edinburg, TX: McAllen Miller International</t>
-  </si>
-  <si>
-    <t>Harlingen/San Benito, TX: Valley International</t>
-  </si>
-  <si>
-    <t>Chattanooga, TN: Lovell Field</t>
-  </si>
-  <si>
-    <t>Missoula, MT: Missoula Montana</t>
-  </si>
-  <si>
-    <t>Kalispell, MT: Glacier Park International</t>
-  </si>
-  <si>
-    <t>Allentown/Bethlehem/Easton, PA: Lehigh Valley International</t>
-  </si>
-  <si>
-    <t>Appleton, WI: Appleton International</t>
-  </si>
-  <si>
-    <t>Atlantic City, NJ: Atlantic City International</t>
-  </si>
-  <si>
-    <t>Jackson, WY: Jackson Hole</t>
-  </si>
-  <si>
-    <t>Tallahassee, FL: Tallahassee International</t>
-  </si>
-  <si>
-    <t>Pasco/Kennewick/Richland, WA: Tri Cities</t>
-  </si>
-  <si>
-    <t>Billings, MT: Billings Logan International</t>
-  </si>
-  <si>
-    <t>Juneau, AK: Juneau International</t>
-  </si>
-  <si>
-    <t>Amarillo, TX: Rick Husband Amarillo International</t>
-  </si>
-  <si>
-    <t>Fort Wayne, IN: Fort Wayne International</t>
-  </si>
-  <si>
-    <t>South Bend, IN: South Bend International</t>
-  </si>
-  <si>
-    <t>New Haven, CT: Tweed New Haven</t>
-  </si>
-  <si>
-    <t>Bangor, ME: Bangor International</t>
-  </si>
-  <si>
-    <t>Rapid City, SD: Rapid City Regional</t>
-  </si>
-  <si>
-    <t>Trenton, NJ: Trenton Mercer</t>
-  </si>
-  <si>
-    <t>Baton Rouge, LA: Baton Rouge Metropolitan/Ryan Field</t>
-  </si>
-  <si>
-    <t>Bellingham, WA: Bellingham International</t>
-  </si>
-  <si>
-    <t>Corpus Christi, TX: Corpus Christi International</t>
-  </si>
-  <si>
-    <t>Idaho Falls, ID: Idaho Falls Regional</t>
-  </si>
-  <si>
-    <t>Santa Rosa, CA: Charles M. Schulz - Sonoma County</t>
-  </si>
-  <si>
-    <t>Aspen, CO: Aspen Pitkin County Sardy Field</t>
-  </si>
-  <si>
-    <t>Flint, MI: Bishop International</t>
-  </si>
-  <si>
-    <t>Roanoke, VA: Roanoke Blacksburg Regional</t>
-  </si>
-  <si>
-    <t>Green Bay, WI: Green Bay Austin Straubel International</t>
-  </si>
-  <si>
-    <t>Traverse City, MI: Cherry Capital</t>
-  </si>
-  <si>
-    <t>Peoria, IL: General Downing - Peoria International</t>
-  </si>
-  <si>
-    <t>Daytona Beach, FL: Daytona Beach International</t>
-  </si>
-  <si>
-    <t>San Luis Obispo, CA: San Luis County Regional</t>
-  </si>
-  <si>
-    <t>Shreveport, LA: Shreveport Regional</t>
-  </si>
-  <si>
-    <t>Moline, IL: Quad Cities International</t>
-  </si>
-  <si>
-    <t>Augusta, GA: Augusta Regional at Bush Field</t>
-  </si>
-  <si>
-    <t>Akron, OH: Akron-Canton Regional</t>
-  </si>
-  <si>
-    <t>Gainesville, FL: Gainesville Regional</t>
-  </si>
-  <si>
-    <t>Mobile, AL: Mobile Regional</t>
-  </si>
-  <si>
-    <t>Everett, WA: Snohomish County</t>
-  </si>
-  <si>
-    <t>Charlottesville, VA: Charlottesville Albemarle</t>
-  </si>
-  <si>
-    <t>Gulfport/Biloxi, MS: Gulfport-Biloxi International</t>
-  </si>
-  <si>
-    <t>Bismarck/Mandan, ND: Bismarck Municipal</t>
-  </si>
-  <si>
-    <t>Montrose/Delta, CO: Montrose Regional</t>
-  </si>
-  <si>
-    <t>Lafayette, LA: Lafayette Regional Paul Fournet Field</t>
-  </si>
-  <si>
-    <t>Monterey, CA: Monterey Regional</t>
-  </si>
-  <si>
-    <t>Grand Junction, CO: Grand Junction Regional</t>
-  </si>
-  <si>
-    <t>Melbourne, FL: Melbourne Orlando International</t>
-  </si>
-  <si>
-    <t>Eagle, CO: Eagle County Regional</t>
-  </si>
-  <si>
-    <t>Provo, UT: Provo Municipal</t>
-  </si>
-  <si>
-    <t>Hayden, CO: Yampa Valley</t>
-  </si>
-  <si>
-    <t>Bristol/Johnson City/Kingsport, TN: Tri Cities</t>
-  </si>
-  <si>
-    <t>Scranton/Wilkes-Barre, PA: Wilkes Barre Scranton International</t>
-  </si>
-  <si>
-    <t>Durango, CO: Durango La Plata County</t>
-  </si>
-  <si>
-    <t>Bloomington/Normal, IL: Central Il Regional Airport at Bloomington</t>
-  </si>
-  <si>
-    <t>Fayetteville, NC: Fayetteville Regional/Grannis Field</t>
-  </si>
-  <si>
-    <t>Charleston/Dunbar, WV: West Virginia International Yeager</t>
-  </si>
-  <si>
-    <t>Belleville, IL: Scott AFB MidAmerica St Louis</t>
-  </si>
-  <si>
-    <t>Evansville, IN: Evansville Regional</t>
-  </si>
-  <si>
-    <t>Montgomery, AL: Montgomery Regional</t>
-  </si>
-  <si>
-    <t>Newburgh/Poughkeepsie, NY: New York Stewart International</t>
-  </si>
-  <si>
-    <t>Columbus, OH: Rickenbacker International</t>
-  </si>
-  <si>
-    <t>Ketchikan, AK: Ketchikan International</t>
-  </si>
-  <si>
-    <t>Great Falls, MT: Great Falls International</t>
-  </si>
-  <si>
-    <t>Bakersfield, CA: Meadows Field</t>
-  </si>
-  <si>
-    <t>Minot, ND: Minot International</t>
-  </si>
-  <si>
-    <t>Jacksonville/Camp Lejeune, NC: Albert J Ellis</t>
-  </si>
-  <si>
-    <t>Nantucket, MA: Nantucket Memorial</t>
-  </si>
-  <si>
-    <t>Bethel, AK: Bethel Airport</t>
-  </si>
-  <si>
-    <t>St. George, UT: St George Regional</t>
-  </si>
-  <si>
-    <t>Source: Bureau of Transportation Statistics, T-100 Market</t>
-  </si>
-  <si>
-    <t>* Systemwide equals domestic plus international</t>
-  </si>
-  <si>
-    <t>Note: Percentage changes based on numbers prior to rounding.</t>
   </si>
 </sst>
 </file>
@@ -726,7 +726,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -756,6 +756,7 @@
     <xf numFmtId="165" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1066,8 +1067,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G204"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:XFD2"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="200" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2494,8 +2495,8 @@
       <c r="A47" s="11">
         <v>46</v>
       </c>
-      <c r="B47" t="s">
-        <v>51</v>
+      <c r="B47" s="15" t="s">
+        <v>208</v>
       </c>
       <c r="C47" s="3">
         <v>4.2222999999999997</v>
@@ -2516,7 +2517,7 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C48" s="3">
         <v>4.1805000000000003</v>
@@ -2537,7 +2538,7 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C49" s="3">
         <v>4.1204999999999998</v>
@@ -2558,7 +2559,7 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C50" s="3">
         <v>3.8875000000000002</v>
@@ -2579,7 +2580,7 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C51" s="3">
         <v>3.6533000000000002</v>
@@ -2600,7 +2601,7 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C52" s="3">
         <v>3.5988000000000002</v>
@@ -2621,7 +2622,7 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C53" s="3">
         <v>3.2456999999999998</v>
@@ -2642,7 +2643,7 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C54" s="3">
         <v>3.1642999999999999</v>
@@ -2663,7 +2664,7 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C55" s="3">
         <v>2.9476</v>
@@ -2684,7 +2685,7 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C56" s="3">
         <v>2.8389000000000002</v>
@@ -2704,8 +2705,8 @@
       <c r="A57" s="11">
         <v>56</v>
       </c>
-      <c r="B57" t="s">
-        <v>61</v>
+      <c r="B57" s="15" t="s">
+        <v>60</v>
       </c>
       <c r="C57" s="3">
         <v>2.8349000000000002</v>
@@ -2726,7 +2727,7 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C58" s="3">
         <v>2.6400999999999999</v>
@@ -2747,7 +2748,7 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C59" s="3">
         <v>2.6049000000000002</v>
@@ -2768,7 +2769,7 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C60" s="3">
         <v>2.4828999999999999</v>
@@ -2789,7 +2790,7 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C61" s="3">
         <v>2.3146</v>
@@ -2810,7 +2811,7 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C62" s="3">
         <v>2.2263999999999999</v>
@@ -2831,7 +2832,7 @@
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C63" s="3">
         <v>2.1972999999999998</v>
@@ -2852,7 +2853,7 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C64" s="3">
         <v>2.1507999999999998</v>
@@ -2873,7 +2874,7 @@
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C65" s="3">
         <v>2.0973000000000002</v>
@@ -2894,7 +2895,7 @@
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C66" s="3">
         <v>2.0609000000000002</v>
@@ -2915,7 +2916,7 @@
         <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C67" s="3">
         <v>2.0337999999999998</v>
@@ -2936,7 +2937,7 @@
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C68" s="3">
         <v>1.9984999999999999</v>
@@ -2957,7 +2958,7 @@
         <v>68</v>
       </c>
       <c r="B69" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C69" s="3">
         <v>1.9941</v>
@@ -2978,7 +2979,7 @@
         <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C70" s="3">
         <v>1.9200999999999999</v>
@@ -2999,7 +3000,7 @@
         <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C71" s="3">
         <v>1.9096</v>
@@ -3020,7 +3021,7 @@
         <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C72" s="3">
         <v>1.9028</v>
@@ -3041,7 +3042,7 @@
         <v>72</v>
       </c>
       <c r="B73" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C73" s="3">
         <v>1.8832</v>
@@ -3062,7 +3063,7 @@
         <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C74" s="3">
         <v>1.8644000000000001</v>
@@ -3083,7 +3084,7 @@
         <v>74</v>
       </c>
       <c r="B75" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C75" s="3">
         <v>1.7645</v>
@@ -3104,7 +3105,7 @@
         <v>75</v>
       </c>
       <c r="B76" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C76" s="3">
         <v>1.7230000000000001</v>
@@ -3125,7 +3126,7 @@
         <v>76</v>
       </c>
       <c r="B77" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C77" s="3">
         <v>1.7129000000000001</v>
@@ -3146,7 +3147,7 @@
         <v>77</v>
       </c>
       <c r="B78" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C78" s="3">
         <v>1.7018</v>
@@ -3167,7 +3168,7 @@
         <v>78</v>
       </c>
       <c r="B79" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C79" s="3">
         <v>1.6918</v>
@@ -3188,7 +3189,7 @@
         <v>79</v>
       </c>
       <c r="B80" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C80" s="3">
         <v>1.5940000000000001</v>
@@ -3209,7 +3210,7 @@
         <v>80</v>
       </c>
       <c r="B81" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C81" s="3">
         <v>1.5640000000000001</v>
@@ -3230,7 +3231,7 @@
         <v>81</v>
       </c>
       <c r="B82" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C82" s="3">
         <v>1.4986999999999999</v>
@@ -3251,7 +3252,7 @@
         <v>82</v>
       </c>
       <c r="B83" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C83" s="3">
         <v>1.4437</v>
@@ -3272,7 +3273,7 @@
         <v>83</v>
       </c>
       <c r="B84" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C84" s="3">
         <v>1.3611</v>
@@ -3293,7 +3294,7 @@
         <v>84</v>
       </c>
       <c r="B85" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C85" s="3">
         <v>1.3599000000000001</v>
@@ -3314,7 +3315,7 @@
         <v>85</v>
       </c>
       <c r="B86" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C86" s="3">
         <v>1.3244</v>
@@ -3335,7 +3336,7 @@
         <v>86</v>
       </c>
       <c r="B87" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C87" s="3">
         <v>1.2755000000000001</v>
@@ -3356,7 +3357,7 @@
         <v>87</v>
       </c>
       <c r="B88" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C88" s="3">
         <v>1.2393000000000001</v>
@@ -3377,7 +3378,7 @@
         <v>88</v>
       </c>
       <c r="B89" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C89" s="3">
         <v>1.2107000000000001</v>
@@ -3398,7 +3399,7 @@
         <v>89</v>
       </c>
       <c r="B90" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C90" s="3">
         <v>1.2099</v>
@@ -3419,7 +3420,7 @@
         <v>90</v>
       </c>
       <c r="B91" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C91" s="3">
         <v>1.2028000000000001</v>
@@ -3440,7 +3441,7 @@
         <v>91</v>
       </c>
       <c r="B92" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C92" s="3">
         <v>1.1553</v>
@@ -3461,7 +3462,7 @@
         <v>92</v>
       </c>
       <c r="B93" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C93" s="3">
         <v>1.1324000000000001</v>
@@ -3482,7 +3483,7 @@
         <v>93</v>
       </c>
       <c r="B94" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C94" s="3">
         <v>1.0744</v>
@@ -3503,7 +3504,7 @@
         <v>94</v>
       </c>
       <c r="B95" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C95" s="3">
         <v>1.0714999999999999</v>
@@ -3524,7 +3525,7 @@
         <v>95</v>
       </c>
       <c r="B96" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C96" s="3">
         <v>1.0641</v>
@@ -3545,7 +3546,7 @@
         <v>96</v>
       </c>
       <c r="B97" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C97" s="3">
         <v>0.98550000000000004</v>
@@ -3566,7 +3567,7 @@
         <v>97</v>
       </c>
       <c r="B98" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C98" s="3">
         <v>0.98170000000000002</v>
@@ -3587,7 +3588,7 @@
         <v>98</v>
       </c>
       <c r="B99" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C99" s="3">
         <v>0.98099999999999998</v>
@@ -3608,7 +3609,7 @@
         <v>99</v>
       </c>
       <c r="B100" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C100" s="3">
         <v>0.94269999999999998</v>
@@ -3629,7 +3630,7 @@
         <v>100</v>
       </c>
       <c r="B101" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C101" s="3">
         <v>0.92049999999999998</v>
@@ -3650,7 +3651,7 @@
         <v>101</v>
       </c>
       <c r="B102" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C102" s="3">
         <v>0.91820000000000002</v>
@@ -3671,7 +3672,7 @@
         <v>102</v>
       </c>
       <c r="B103" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C103" s="3">
         <v>0.90859999999999996</v>
@@ -3692,7 +3693,7 @@
         <v>103</v>
       </c>
       <c r="B104" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C104" s="3">
         <v>0.89200000000000002</v>
@@ -3713,7 +3714,7 @@
         <v>104</v>
       </c>
       <c r="B105" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C105" s="3">
         <v>0.80840000000000001</v>
@@ -3734,7 +3735,7 @@
         <v>105</v>
       </c>
       <c r="B106" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C106" s="3">
         <v>0.78269999999999995</v>
@@ -3755,7 +3756,7 @@
         <v>106</v>
       </c>
       <c r="B107" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C107" s="3">
         <v>0.77649999999999997</v>
@@ -3776,7 +3777,7 @@
         <v>107</v>
       </c>
       <c r="B108" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C108" s="3">
         <v>0.75880000000000003</v>
@@ -3797,7 +3798,7 @@
         <v>108</v>
       </c>
       <c r="B109" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C109" s="3">
         <v>0.74619999999999997</v>
@@ -3818,7 +3819,7 @@
         <v>109</v>
       </c>
       <c r="B110" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C110" s="3">
         <v>0.69259999999999999</v>
@@ -3839,7 +3840,7 @@
         <v>110</v>
       </c>
       <c r="B111" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C111" s="3">
         <v>0.64280000000000004</v>
@@ -3860,7 +3861,7 @@
         <v>111</v>
       </c>
       <c r="B112" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C112" s="3">
         <v>0.63619999999999999</v>
@@ -3881,7 +3882,7 @@
         <v>112</v>
       </c>
       <c r="B113" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C113" s="3">
         <v>0.63260000000000005</v>
@@ -3902,7 +3903,7 @@
         <v>113</v>
       </c>
       <c r="B114" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C114" s="3">
         <v>0.6179</v>
@@ -3923,7 +3924,7 @@
         <v>114</v>
       </c>
       <c r="B115" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C115" s="3">
         <v>0.61040000000000005</v>
@@ -3944,7 +3945,7 @@
         <v>115</v>
       </c>
       <c r="B116" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C116" s="3">
         <v>0.60970000000000002</v>
@@ -3965,7 +3966,7 @@
         <v>116</v>
       </c>
       <c r="B117" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C117" s="3">
         <v>0.60570000000000002</v>
@@ -3986,7 +3987,7 @@
         <v>117</v>
       </c>
       <c r="B118" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C118" s="3">
         <v>0.60189999999999999</v>
@@ -4007,7 +4008,7 @@
         <v>118</v>
       </c>
       <c r="B119" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C119" s="3">
         <v>0.6008</v>
@@ -4028,7 +4029,7 @@
         <v>119</v>
       </c>
       <c r="B120" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C120" s="3">
         <v>0.59760000000000002</v>
@@ -4049,7 +4050,7 @@
         <v>120</v>
       </c>
       <c r="B121" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C121" s="3">
         <v>0.58679999999999999</v>
@@ -4070,7 +4071,7 @@
         <v>121</v>
       </c>
       <c r="B122" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C122" s="3">
         <v>0.57150000000000001</v>
@@ -4091,7 +4092,7 @@
         <v>122</v>
       </c>
       <c r="B123" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C123" s="3">
         <v>0.55530000000000002</v>
@@ -4112,7 +4113,7 @@
         <v>123</v>
       </c>
       <c r="B124" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C124" s="3">
         <v>0.53720000000000001</v>
@@ -4133,7 +4134,7 @@
         <v>124</v>
       </c>
       <c r="B125" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C125" s="3">
         <v>0.53520000000000001</v>
@@ -4154,7 +4155,7 @@
         <v>125</v>
       </c>
       <c r="B126" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C126" s="3">
         <v>0.51280000000000003</v>
@@ -4175,7 +4176,7 @@
         <v>126</v>
       </c>
       <c r="B127" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C127" s="3">
         <v>0.50380000000000003</v>
@@ -4196,7 +4197,7 @@
         <v>127</v>
       </c>
       <c r="B128" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C128" s="3">
         <v>0.50029999999999997</v>
@@ -4217,7 +4218,7 @@
         <v>128</v>
       </c>
       <c r="B129" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C129" s="3">
         <v>0.49890000000000001</v>
@@ -4238,7 +4239,7 @@
         <v>129</v>
       </c>
       <c r="B130" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C130" s="3">
         <v>0.4854</v>
@@ -4259,7 +4260,7 @@
         <v>130</v>
       </c>
       <c r="B131" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C131" s="3">
         <v>0.4572</v>
@@ -4280,7 +4281,7 @@
         <v>131</v>
       </c>
       <c r="B132" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C132" s="3">
         <v>0.44779999999999998</v>
@@ -4301,7 +4302,7 @@
         <v>132</v>
       </c>
       <c r="B133" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C133" s="3">
         <v>0.4325</v>
@@ -4322,7 +4323,7 @@
         <v>133</v>
       </c>
       <c r="B134" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C134" s="3">
         <v>0.42949999999999999</v>
@@ -4343,7 +4344,7 @@
         <v>134</v>
       </c>
       <c r="B135" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C135" s="3">
         <v>0.42349999999999999</v>
@@ -4364,7 +4365,7 @@
         <v>135</v>
       </c>
       <c r="B136" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C136" s="3">
         <v>0.4204</v>
@@ -4385,7 +4386,7 @@
         <v>136</v>
       </c>
       <c r="B137" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C137" s="3">
         <v>0.41860000000000003</v>
@@ -4406,7 +4407,7 @@
         <v>137</v>
       </c>
       <c r="B138" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C138" s="3">
         <v>0.41539999999999999</v>
@@ -4427,7 +4428,7 @@
         <v>138</v>
       </c>
       <c r="B139" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C139" s="3">
         <v>0.41160000000000002</v>
@@ -4448,7 +4449,7 @@
         <v>139</v>
       </c>
       <c r="B140" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C140" s="3">
         <v>0.3992</v>
@@ -4469,7 +4470,7 @@
         <v>140</v>
       </c>
       <c r="B141" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C141" s="3">
         <v>0.39290000000000003</v>
@@ -4489,8 +4490,8 @@
       <c r="A142" s="11">
         <v>141</v>
       </c>
-      <c r="B142" t="s">
-        <v>146</v>
+      <c r="B142" s="15" t="s">
+        <v>206</v>
       </c>
       <c r="C142" s="3">
         <v>0.39040000000000002</v>
@@ -4511,7 +4512,7 @@
         <v>142</v>
       </c>
       <c r="B143" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C143" s="3">
         <v>0.38640000000000002</v>
@@ -4532,7 +4533,7 @@
         <v>143</v>
       </c>
       <c r="B144" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C144" s="3">
         <v>0.35930000000000001</v>
@@ -4553,7 +4554,7 @@
         <v>144</v>
       </c>
       <c r="B145" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C145" s="3">
         <v>0.35830000000000001</v>
@@ -4574,7 +4575,7 @@
         <v>145</v>
       </c>
       <c r="B146" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C146" s="3">
         <v>0.35730000000000001</v>
@@ -4595,7 +4596,7 @@
         <v>146</v>
       </c>
       <c r="B147" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C147" s="3">
         <v>0.35709999999999997</v>
@@ -4616,7 +4617,7 @@
         <v>147</v>
       </c>
       <c r="B148" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C148" s="3">
         <v>0.34329999999999999</v>
@@ -4637,7 +4638,7 @@
         <v>148</v>
       </c>
       <c r="B149" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C149" s="3">
         <v>0.33689999999999998</v>
@@ -4658,7 +4659,7 @@
         <v>149</v>
       </c>
       <c r="B150" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C150" s="3">
         <v>0.33069999999999999</v>
@@ -4679,7 +4680,7 @@
         <v>150</v>
       </c>
       <c r="B151" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C151" s="3">
         <v>0.3281</v>
@@ -4700,7 +4701,7 @@
         <v>151</v>
       </c>
       <c r="B152" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C152" s="3">
         <v>0.32640000000000002</v>
@@ -4721,7 +4722,7 @@
         <v>152</v>
       </c>
       <c r="B153" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C153" s="3">
         <v>0.32029999999999997</v>
@@ -4742,7 +4743,7 @@
         <v>153</v>
       </c>
       <c r="B154" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C154" s="3">
         <v>0.31709999999999999</v>
@@ -4763,7 +4764,7 @@
         <v>154</v>
       </c>
       <c r="B155" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C155" s="3">
         <v>0.30840000000000001</v>
@@ -4784,7 +4785,7 @@
         <v>155</v>
       </c>
       <c r="B156" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C156" s="3">
         <v>0.30349999999999999</v>
@@ -4805,7 +4806,7 @@
         <v>156</v>
       </c>
       <c r="B157" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C157" s="3">
         <v>0.29880000000000001</v>
@@ -4826,7 +4827,7 @@
         <v>157</v>
       </c>
       <c r="B158" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C158" s="3">
         <v>0.29849999999999999</v>
@@ -4847,7 +4848,7 @@
         <v>158</v>
       </c>
       <c r="B159" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C159" s="3">
         <v>0.29680000000000001</v>
@@ -4868,7 +4869,7 @@
         <v>159</v>
       </c>
       <c r="B160" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C160" s="3">
         <v>0.29409999999999997</v>
@@ -4889,7 +4890,7 @@
         <v>160</v>
       </c>
       <c r="B161" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C161" s="3">
         <v>0.2878</v>
@@ -4910,7 +4911,7 @@
         <v>161</v>
       </c>
       <c r="B162" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C162" s="3">
         <v>0.28320000000000001</v>
@@ -4931,7 +4932,7 @@
         <v>162</v>
       </c>
       <c r="B163" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C163" s="3">
         <v>0.2782</v>
@@ -4952,7 +4953,7 @@
         <v>163</v>
       </c>
       <c r="B164" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C164" s="3">
         <v>0.27250000000000002</v>
@@ -4973,7 +4974,7 @@
         <v>164</v>
       </c>
       <c r="B165" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C165" s="3">
         <v>0.2717</v>
@@ -4994,7 +4995,7 @@
         <v>165</v>
       </c>
       <c r="B166" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C166" s="3">
         <v>0.26769999999999999</v>
@@ -5015,7 +5016,7 @@
         <v>166</v>
       </c>
       <c r="B167" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C167" s="3">
         <v>0.2676</v>
@@ -5036,7 +5037,7 @@
         <v>167</v>
       </c>
       <c r="B168" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C168" s="3">
         <v>0.26179999999999998</v>
@@ -5057,7 +5058,7 @@
         <v>168</v>
       </c>
       <c r="B169" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C169" s="3">
         <v>0.26179999999999998</v>
@@ -5078,7 +5079,7 @@
         <v>169</v>
       </c>
       <c r="B170" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C170" s="3">
         <v>0.26150000000000001</v>
@@ -5099,7 +5100,7 @@
         <v>170</v>
       </c>
       <c r="B171" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C171" s="3">
         <v>0.26040000000000002</v>
@@ -5120,7 +5121,7 @@
         <v>171</v>
       </c>
       <c r="B172" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C172" s="3">
         <v>0.25979999999999998</v>
@@ -5141,7 +5142,7 @@
         <v>172</v>
       </c>
       <c r="B173" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C173" s="3">
         <v>0.2437</v>
@@ -5162,7 +5163,7 @@
         <v>173</v>
       </c>
       <c r="B174" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C174" s="3">
         <v>0.2417</v>
@@ -5183,7 +5184,7 @@
         <v>174</v>
       </c>
       <c r="B175" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C175" s="3">
         <v>0.23269999999999999</v>
@@ -5204,7 +5205,7 @@
         <v>175</v>
       </c>
       <c r="B176" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C176" s="3">
         <v>0.22450000000000001</v>
@@ -5225,7 +5226,7 @@
         <v>176</v>
       </c>
       <c r="B177" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C177" s="3">
         <v>0.22420000000000001</v>
@@ -5246,7 +5247,7 @@
         <v>177</v>
       </c>
       <c r="B178" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C178" s="3">
         <v>0.22140000000000001</v>
@@ -5267,7 +5268,7 @@
         <v>178</v>
       </c>
       <c r="B179" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C179" s="3">
         <v>0.2185</v>
@@ -5288,7 +5289,7 @@
         <v>179</v>
       </c>
       <c r="B180" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C180" s="3">
         <v>0.2145</v>
@@ -5309,7 +5310,7 @@
         <v>180</v>
       </c>
       <c r="B181" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C181" s="3">
         <v>0.20860000000000001</v>
@@ -5330,7 +5331,7 @@
         <v>181</v>
       </c>
       <c r="B182" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C182" s="3">
         <v>0.19689999999999999</v>
@@ -5350,8 +5351,8 @@
       <c r="A183" s="11">
         <v>182</v>
       </c>
-      <c r="B183" t="s">
-        <v>187</v>
+      <c r="B183" s="15" t="s">
+        <v>207</v>
       </c>
       <c r="C183" s="3">
         <v>0.19109999999999999</v>
@@ -5372,7 +5373,7 @@
         <v>183</v>
       </c>
       <c r="B184" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C184" s="3">
         <v>0.18859999999999999</v>
@@ -5393,7 +5394,7 @@
         <v>184</v>
       </c>
       <c r="B185" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C185" s="3">
         <v>0.18329999999999999</v>
@@ -5414,7 +5415,7 @@
         <v>185</v>
       </c>
       <c r="B186" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C186" s="3">
         <v>0.17330000000000001</v>
@@ -5435,7 +5436,7 @@
         <v>186</v>
       </c>
       <c r="B187" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C187" s="3">
         <v>0.16450000000000001</v>
@@ -5456,7 +5457,7 @@
         <v>187</v>
       </c>
       <c r="B188" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="C188" s="3">
         <v>0.1638</v>
@@ -5477,7 +5478,7 @@
         <v>188</v>
       </c>
       <c r="B189" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="C189" s="3">
         <v>0.16259999999999999</v>
@@ -5498,7 +5499,7 @@
         <v>189</v>
       </c>
       <c r="B190" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C190" s="3">
         <v>0.15260000000000001</v>
@@ -5519,7 +5520,7 @@
         <v>190</v>
       </c>
       <c r="B191" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="C191" s="3">
         <v>0.1507</v>
@@ -5540,7 +5541,7 @@
         <v>191</v>
       </c>
       <c r="B192" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="C192" s="3">
         <v>0.1497</v>
@@ -5561,7 +5562,7 @@
         <v>192</v>
       </c>
       <c r="B193" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C193" s="3">
         <v>0.14699999999999999</v>
@@ -5582,7 +5583,7 @@
         <v>193</v>
       </c>
       <c r="B194" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="C194" s="3">
         <v>0.14269999999999999</v>
@@ -5603,7 +5604,7 @@
         <v>194</v>
       </c>
       <c r="B195" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C195" s="3">
         <v>0.14099999999999999</v>
@@ -5624,7 +5625,7 @@
         <v>195</v>
       </c>
       <c r="B196" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C196" s="3">
         <v>0.1409</v>
@@ -5645,7 +5646,7 @@
         <v>196</v>
       </c>
       <c r="B197" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="C197" s="3">
         <v>0.13869999999999999</v>
@@ -5666,7 +5667,7 @@
         <v>197</v>
       </c>
       <c r="B198" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="C198" s="3">
         <v>0.13689999999999999</v>
@@ -5687,7 +5688,7 @@
         <v>198</v>
       </c>
       <c r="B199" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="C199" s="3">
         <v>0.13650000000000001</v>
@@ -5708,7 +5709,7 @@
         <v>199</v>
       </c>
       <c r="B200" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C200" s="3">
         <v>0.1356</v>
@@ -5729,7 +5730,7 @@
         <v>200</v>
       </c>
       <c r="B201" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C201" s="3">
         <v>0.12740000000000001</v>
@@ -5746,34 +5747,34 @@
       <c r="G201"/>
     </row>
     <row r="202" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A202" s="15" t="s">
-        <v>206</v>
-      </c>
-      <c r="B202" s="15"/>
-      <c r="C202" s="15"/>
-      <c r="D202" s="15"/>
-      <c r="E202" s="15"/>
-      <c r="F202" s="15"/>
+      <c r="A202" s="16" t="s">
+        <v>203</v>
+      </c>
+      <c r="B202" s="16"/>
+      <c r="C202" s="16"/>
+      <c r="D202" s="16"/>
+      <c r="E202" s="16"/>
+      <c r="F202" s="16"/>
     </row>
     <row r="203" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A203" s="16" t="s">
-        <v>207</v>
-      </c>
-      <c r="B203" s="17"/>
-      <c r="C203" s="17"/>
-      <c r="D203" s="17"/>
-      <c r="E203" s="17"/>
-      <c r="F203" s="17"/>
+      <c r="A203" s="17" t="s">
+        <v>204</v>
+      </c>
+      <c r="B203" s="18"/>
+      <c r="C203" s="18"/>
+      <c r="D203" s="18"/>
+      <c r="E203" s="18"/>
+      <c r="F203" s="18"/>
     </row>
     <row r="204" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A204" s="17" t="s">
-        <v>208</v>
-      </c>
-      <c r="B204" s="17"/>
-      <c r="C204" s="17"/>
-      <c r="D204" s="17"/>
-      <c r="E204" s="17"/>
-      <c r="F204" s="17"/>
+      <c r="A204" s="18" t="s">
+        <v>205</v>
+      </c>
+      <c r="B204" s="18"/>
+      <c r="C204" s="18"/>
+      <c r="D204" s="18"/>
+      <c r="E204" s="18"/>
+      <c r="F204" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>